<commit_message>
added to class 1
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/063f9107f230d788/idos_shit/Tel_Hai_GIS_ecology_24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6DD17CF-B0B4-43C4-AEFF-F45F5D412570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C6DD17CF-B0B4-43C4-AEFF-F45F5D412570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06690BD2-47A0-4A80-93EE-58A4DE8F2A7B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67C54D80-F925-4475-9AE8-30A92D946929}"/>
+    <workbookView xWindow="3375" yWindow="3030" windowWidth="18900" windowHeight="10965" xr2:uid="{67C54D80-F925-4475-9AE8-30A92D946929}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>?</t>
   </si>
   <si>
-    <t xml:space="preserve">תרגיל חדש - </t>
-  </si>
-  <si>
     <t>מ</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>הצגת התרגיל המסכם</t>
+  </si>
+  <si>
+    <t>תרגיל חדש -  פרופיל גבהים</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,10 +614,10 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -628,16 +628,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -654,10 +654,10 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
         <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,13 +691,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -711,13 +711,13 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -731,13 +731,13 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -751,13 +751,13 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -768,16 +768,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -788,16 +788,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,10 +814,10 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -831,10 +831,10 @@
         <v>23</v>
       </c>
       <c r="H12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" t="s">
         <v>37</v>
-      </c>
-      <c r="I12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -845,16 +845,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -862,16 +862,16 @@
         <v>45390</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
         <v>58</v>
-      </c>
-      <c r="I14" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -885,26 +885,26 @@
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -912,10 +912,10 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -935,37 +935,37 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>